<commit_message>
Updates to L09 and peer feed back assignment
</commit_message>
<xml_diff>
--- a/projects/Data Project - peer assignment.xlsx
+++ b/projects/Data Project - peer assignment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="48">
   <si>
     <t>team</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Numpy</t>
-  </si>
-  <si>
-    <t>The-Danish-German-Alliance</t>
   </si>
   <si>
     <t>a12</t>
@@ -518,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -771,10 +768,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -782,10 +779,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -793,10 +790,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -804,10 +801,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -815,10 +812,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -826,10 +823,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -837,10 +834,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -848,10 +845,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -859,10 +856,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -870,10 +867,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -881,7 +878,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
@@ -892,10 +889,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -903,10 +900,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -914,10 +911,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -925,10 +922,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -936,10 +933,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -947,10 +944,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -958,10 +955,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -969,10 +966,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -983,7 +980,7 @@
         <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -991,10 +988,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1002,10 +999,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1013,10 +1010,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1024,21 +1021,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>